<commit_message>
Use a more robust IF check in the formulas
Fixes #409
In the formulas in columns D, F and G the IF conditions are changed
from E9=0 to A9="", to be able to handle very short segments where the
horizontal distance rounds down to 0.
In the formulas in column K, the IF condition is removed entirely,
because this condition isn't required for the correct behaviour, and it
caused the planned time of arrival to be reset to zero in edge cases.
</commit_message>
<xml_diff>
--- a/backend/automatic_walk_time_tables/res/Marschzeit_Template.xlsx
+++ b/backend/automatic_walk_time_tables/res/Marschzeit_Template.xlsx
@@ -641,7 +641,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -831,11 +831,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2241567"/>
-        <c:axId val="78022108"/>
+        <c:axId val="19138306"/>
+        <c:axId val="56054005"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2241567"/>
+        <c:axId val="19138306"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -912,13 +912,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78022108"/>
+        <c:crossAx val="56054005"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78022108"/>
+        <c:axId val="56054005"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -994,7 +994,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2241567"/>
+        <c:crossAx val="19138306"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1035,9 +1035,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1511640</xdr:colOff>
+      <xdr:colOff>1510920</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1046,7 +1046,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="92880" y="12351600"/>
-        <a:ext cx="12729240" cy="4041000"/>
+        <a:ext cx="10392480" cy="4040280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1065,9 +1065,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1887480</xdr:colOff>
+      <xdr:colOff>1886760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>758880</xdr:rowOff>
+      <xdr:rowOff>758160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1080,8 +1080,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12598560" y="145080"/>
-          <a:ext cx="599400" cy="613800"/>
+          <a:off x="10262520" y="145080"/>
+          <a:ext cx="598680" cy="613080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1102,9 +1102,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1189080</xdr:colOff>
+      <xdr:colOff>1188360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>817560</xdr:rowOff>
+      <xdr:rowOff>816840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1117,8 +1117,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8942400" y="140400"/>
-          <a:ext cx="3557160" cy="677160"/>
+          <a:off x="7215840" y="140400"/>
+          <a:ext cx="2946960" cy="676440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1141,10 +1141,10 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T6" activeCellId="0" sqref="T6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="3" style="0" width="8.29"/>
@@ -1361,16 +1361,16 @@
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="31" t="n">
-        <f aca="false">IF(E9=0,0,IF(C9&gt;0,(C9-C8)/100,0))</f>
+        <f aca="false">IF(A9="",0,IF(C9&gt;0,(C9-C8)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="33" t="n">
-        <f aca="false">IF(E9=0,0,IF(J9&lt;-20,-D9/1.5+E9,IF(J9&lt;0,E9,D9+E9)))</f>
+        <f aca="false">IF(A9="",0,IF(J9&lt;-20,-D9/1.5+E9,IF(J9&lt;0,E9,D9+E9)))</f>
         <v>0</v>
       </c>
       <c r="G9" s="34" t="n">
-        <f aca="false">IF(E9=0,0,TIME(0,60/$N$3*F9,0))</f>
+        <f aca="false">IF(A9="",0,TIME(0,60/$N$3*F9,0))</f>
         <v>0</v>
       </c>
       <c r="H9" s="33" t="n">
@@ -1386,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="35" t="n">
-        <f aca="false">IF((K8+G9+M9)&lt;&gt;K8,K8+G9+M9,0)</f>
+        <f aca="false">K8+G9+M9</f>
         <v>0</v>
       </c>
       <c r="L9" s="28"/>
@@ -1398,16 +1398,16 @@
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
       <c r="D10" s="31" t="n">
-        <f aca="false">IF(E10=0,0,IF(C10&gt;0,(C10-C9)/100,0))</f>
+        <f aca="false">IF(A10="",0,IF(C10&gt;0,(C10-C9)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="33" t="n">
-        <f aca="false">IF(E10=0,0,IF(J10&lt;-20,-D10/1.5+E10,IF(J10&lt;0,E10,D10+E10)))</f>
+        <f aca="false">IF(A10="",0,IF(J10&lt;-20,-D10/1.5+E10,IF(J10&lt;0,E10,D10+E10)))</f>
         <v>0</v>
       </c>
       <c r="G10" s="34" t="n">
-        <f aca="false">IF(E10=0,0,TIME(0,60/$N$3*F10,0))</f>
+        <f aca="false">IF(A10="",0,TIME(0,60/$N$3*F10,0))</f>
         <v>0</v>
       </c>
       <c r="H10" s="33" t="n">
@@ -1423,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="35" t="n">
-        <f aca="false">IF((K9+G10+M10)&lt;&gt;K9,K9+G10+M10,0)</f>
+        <f aca="false">K9+G10+M10</f>
         <v>0</v>
       </c>
       <c r="L10" s="28"/>
@@ -1435,16 +1435,16 @@
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
       <c r="D11" s="31" t="n">
-        <f aca="false">IF(E11=0,0,IF(C11&gt;0,(C11-C10)/100,0))</f>
+        <f aca="false">IF(A11="",0,IF(C11&gt;0,(C11-C10)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="33" t="n">
-        <f aca="false">IF(E11=0,0,IF(J11&lt;-20,-D11/1.5+E11,IF(J11&lt;0,E11,D11+E11)))</f>
+        <f aca="false">IF(A11="",0,IF(J11&lt;-20,-D11/1.5+E11,IF(J11&lt;0,E11,D11+E11)))</f>
         <v>0</v>
       </c>
       <c r="G11" s="34" t="n">
-        <f aca="false">IF(E11=0,0,TIME(0,60/$N$3*F11,0))</f>
+        <f aca="false">IF(A11="",0,TIME(0,60/$N$3*F11,0))</f>
         <v>0</v>
       </c>
       <c r="H11" s="33" t="n">
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="35" t="n">
-        <f aca="false">IF((K10+G11+M11)&lt;&gt;K10,K10+G11+M11,0)</f>
+        <f aca="false">K10+G11+M11</f>
         <v>0</v>
       </c>
       <c r="L11" s="28"/>
@@ -1472,16 +1472,16 @@
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
       <c r="D12" s="31" t="n">
-        <f aca="false">IF(E12=0,0,IF(C12&gt;0,(C12-C11)/100,0))</f>
+        <f aca="false">IF(A12="",0,IF(C12&gt;0,(C12-C11)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="33" t="n">
-        <f aca="false">IF(E12=0,0,IF(J12&lt;-20,-D12/1.5+E12,IF(J12&lt;0,E12,D12+E12)))</f>
+        <f aca="false">IF(A12="",0,IF(J12&lt;-20,-D12/1.5+E12,IF(J12&lt;0,E12,D12+E12)))</f>
         <v>0</v>
       </c>
       <c r="G12" s="34" t="n">
-        <f aca="false">IF(E12=0,0,TIME(0,60/$N$3*F12,0))</f>
+        <f aca="false">IF(A12="",0,TIME(0,60/$N$3*F12,0))</f>
         <v>0</v>
       </c>
       <c r="H12" s="33" t="n">
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="35" t="n">
-        <f aca="false">IF((K11+G12+M12)&lt;&gt;K11,K11+G12+M12,0)</f>
+        <f aca="false">K11+G12+M12</f>
         <v>0</v>
       </c>
       <c r="L12" s="28"/>
@@ -1509,16 +1509,16 @@
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
       <c r="D13" s="31" t="n">
-        <f aca="false">IF(E13=0,0,IF(C13&gt;0,(C13-C12)/100,0))</f>
+        <f aca="false">IF(A13="",0,IF(C13&gt;0,(C13-C12)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="33" t="n">
-        <f aca="false">IF(E13=0,0,IF(J13&lt;-20,-D13/1.5+E13,IF(J13&lt;0,E13,D13+E13)))</f>
+        <f aca="false">IF(A13="",0,IF(J13&lt;-20,-D13/1.5+E13,IF(J13&lt;0,E13,D13+E13)))</f>
         <v>0</v>
       </c>
       <c r="G13" s="34" t="n">
-        <f aca="false">IF(E13=0,0,TIME(0,60/$N$3*F13,0))</f>
+        <f aca="false">IF(A13="",0,TIME(0,60/$N$3*F13,0))</f>
         <v>0</v>
       </c>
       <c r="H13" s="33" t="n">
@@ -1534,7 +1534,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="35" t="n">
-        <f aca="false">IF((K12+G13+M13)&lt;&gt;K12,K12+G13+M13,0)</f>
+        <f aca="false">K12+G13+M13</f>
         <v>0</v>
       </c>
       <c r="L13" s="28"/>
@@ -1546,16 +1546,16 @@
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
       <c r="D14" s="31" t="n">
-        <f aca="false">IF(E14=0,0,IF(C14&gt;0,(C14-C13)/100,0))</f>
+        <f aca="false">IF(A14="",0,IF(C14&gt;0,(C14-C13)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E14" s="36"/>
       <c r="F14" s="33" t="n">
-        <f aca="false">IF(E14=0,0,IF(J14&lt;-20,-D14/1.5+E14,IF(J14&lt;0,E14,D14+E14)))</f>
+        <f aca="false">IF(A14="",0,IF(J14&lt;-20,-D14/1.5+E14,IF(J14&lt;0,E14,D14+E14)))</f>
         <v>0</v>
       </c>
       <c r="G14" s="34" t="n">
-        <f aca="false">IF(E14=0,0,TIME(0,60/$N$3*F14,0))</f>
+        <f aca="false">IF(A14="",0,TIME(0,60/$N$3*F14,0))</f>
         <v>0</v>
       </c>
       <c r="H14" s="33" t="n">
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="35" t="n">
-        <f aca="false">IF((K13+G14+M14)&lt;&gt;K13,K13+G14+M14,0)</f>
+        <f aca="false">K13+G14+M14</f>
         <v>0</v>
       </c>
       <c r="L14" s="28"/>
@@ -1583,16 +1583,16 @@
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
       <c r="D15" s="31" t="n">
-        <f aca="false">IF(E15=0,0,IF(C15&gt;0,(C15-C14)/100,0))</f>
+        <f aca="false">IF(A15="",0,IF(C15&gt;0,(C15-C14)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="33" t="n">
-        <f aca="false">IF(E15=0,0,IF(J15&lt;-20,-D15/1.5+E15,IF(J15&lt;0,E15,D15+E15)))</f>
+        <f aca="false">IF(A15="",0,IF(J15&lt;-20,-D15/1.5+E15,IF(J15&lt;0,E15,D15+E15)))</f>
         <v>0</v>
       </c>
       <c r="G15" s="34" t="n">
-        <f aca="false">IF(E15=0,0,TIME(0,60/$N$3*F15,0))</f>
+        <f aca="false">IF(A15="",0,TIME(0,60/$N$3*F15,0))</f>
         <v>0</v>
       </c>
       <c r="H15" s="33" t="n">
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="35" t="n">
-        <f aca="false">IF((K14+G15+M15)&lt;&gt;K14,K14+G15+M15,0)</f>
+        <f aca="false">K14+G15+M15</f>
         <v>0</v>
       </c>
       <c r="L15" s="28"/>
@@ -1620,16 +1620,16 @@
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
       <c r="D16" s="31" t="n">
-        <f aca="false">IF(E16=0,0,IF(C16&gt;0,(C16-C15)/100,0))</f>
+        <f aca="false">IF(A16="",0,IF(C16&gt;0,(C16-C15)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E16" s="36"/>
       <c r="F16" s="33" t="n">
-        <f aca="false">IF(E16=0,0,IF(J16&lt;-20,-D16/1.5+E16,IF(J16&lt;0,E16,D16+E16)))</f>
+        <f aca="false">IF(A16="",0,IF(J16&lt;-20,-D16/1.5+E16,IF(J16&lt;0,E16,D16+E16)))</f>
         <v>0</v>
       </c>
       <c r="G16" s="34" t="n">
-        <f aca="false">IF(E16=0,0,TIME(0,60/$N$3*F16,0))</f>
+        <f aca="false">IF(A16="",0,TIME(0,60/$N$3*F16,0))</f>
         <v>0</v>
       </c>
       <c r="H16" s="33" t="n">
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="K16" s="35" t="n">
-        <f aca="false">IF((K15+G16+M16)&lt;&gt;K15,K15+G16+M16,0)</f>
+        <f aca="false">K15+G16+M16</f>
         <v>0</v>
       </c>
       <c r="L16" s="28"/>
@@ -1657,16 +1657,16 @@
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
       <c r="D17" s="31" t="n">
-        <f aca="false">IF(E17=0,0,IF(C17&gt;0,(C17-C16)/100,0))</f>
+        <f aca="false">IF(A17="",0,IF(C17&gt;0,(C17-C16)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E17" s="36"/>
       <c r="F17" s="33" t="n">
-        <f aca="false">IF(E17=0,0,IF(J17&lt;-20,-D17/1.5+E17,IF(J17&lt;0,E17,D17+E17)))</f>
+        <f aca="false">IF(A17="",0,IF(J17&lt;-20,-D17/1.5+E17,IF(J17&lt;0,E17,D17+E17)))</f>
         <v>0</v>
       </c>
       <c r="G17" s="34" t="n">
-        <f aca="false">IF(E17=0,0,TIME(0,60/$N$3*F17,0))</f>
+        <f aca="false">IF(A17="",0,TIME(0,60/$N$3*F17,0))</f>
         <v>0</v>
       </c>
       <c r="H17" s="33" t="n">
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="K17" s="35" t="n">
-        <f aca="false">IF((K16+G17+M17)&lt;&gt;K16,K16+G17+M17,0)</f>
+        <f aca="false">K16+G17+M17</f>
         <v>0</v>
       </c>
       <c r="L17" s="28"/>
@@ -1694,16 +1694,16 @@
       <c r="B18" s="23"/>
       <c r="C18" s="24"/>
       <c r="D18" s="31" t="n">
-        <f aca="false">IF(E18=0,0,IF(C18&gt;0,(C18-C17)/100,0))</f>
+        <f aca="false">IF(A18="",0,IF(C18&gt;0,(C18-C17)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="33" t="n">
-        <f aca="false">IF(E18=0,0,IF(J18&lt;-20,-D18/1.5+E18,IF(J18&lt;0,E18,D18+E18)))</f>
+        <f aca="false">IF(A18="",0,IF(J18&lt;-20,-D18/1.5+E18,IF(J18&lt;0,E18,D18+E18)))</f>
         <v>0</v>
       </c>
       <c r="G18" s="34" t="n">
-        <f aca="false">IF(E18=0,0,TIME(0,60/$N$3*F18,0))</f>
+        <f aca="false">IF(A18="",0,TIME(0,60/$N$3*F18,0))</f>
         <v>0</v>
       </c>
       <c r="H18" s="33" t="n">
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="35" t="n">
-        <f aca="false">IF((K17+G18+M18)&lt;&gt;K17,K17+G18+M18,0)</f>
+        <f aca="false">K17+G18+M18</f>
         <v>0</v>
       </c>
       <c r="L18" s="28"/>
@@ -1731,16 +1731,16 @@
       <c r="B19" s="23"/>
       <c r="C19" s="24"/>
       <c r="D19" s="31" t="n">
-        <f aca="false">IF(E19=0,0,IF(C19&gt;0,(C19-C18)/100,0))</f>
+        <f aca="false">IF(A19="",0,IF(C19&gt;0,(C19-C18)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="33" t="n">
-        <f aca="false">IF(E19=0,0,IF(J19&lt;-20,-D19/1.5+E19,IF(J19&lt;0,E19,D19+E19)))</f>
+        <f aca="false">IF(A19="",0,IF(J19&lt;-20,-D19/1.5+E19,IF(J19&lt;0,E19,D19+E19)))</f>
         <v>0</v>
       </c>
       <c r="G19" s="34" t="n">
-        <f aca="false">IF(E19=0,0,TIME(0,60/$N$3*F19,0))</f>
+        <f aca="false">IF(A19="",0,TIME(0,60/$N$3*F19,0))</f>
         <v>0</v>
       </c>
       <c r="H19" s="33" t="n">
@@ -1756,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="35" t="n">
-        <f aca="false">IF((K18+G19+M19)&lt;&gt;K18,K18+G19+M19,0)</f>
+        <f aca="false">K18+G19+M19</f>
         <v>0</v>
       </c>
       <c r="L19" s="37"/>
@@ -1768,16 +1768,16 @@
       <c r="B20" s="23"/>
       <c r="C20" s="24"/>
       <c r="D20" s="31" t="n">
-        <f aca="false">IF(E20=0,0,IF(C20&gt;0,(C20-C19)/100,0))</f>
+        <f aca="false">IF(A20="",0,IF(C20&gt;0,(C20-C19)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E20" s="36"/>
       <c r="F20" s="33" t="n">
-        <f aca="false">IF(E20=0,0,IF(J20&lt;-20,-D20/1.5+E20,IF(J20&lt;0,E20,D20+E20)))</f>
+        <f aca="false">IF(A20="",0,IF(J20&lt;-20,-D20/1.5+E20,IF(J20&lt;0,E20,D20+E20)))</f>
         <v>0</v>
       </c>
       <c r="G20" s="34" t="n">
-        <f aca="false">IF(E20=0,0,TIME(0,60/$N$3*F20,0))</f>
+        <f aca="false">IF(A20="",0,TIME(0,60/$N$3*F20,0))</f>
         <v>0</v>
       </c>
       <c r="H20" s="33" t="n">
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="35" t="n">
-        <f aca="false">IF((K19+G20+M20)&lt;&gt;K19,K19+G20+M20,0)</f>
+        <f aca="false">K19+G20+M20</f>
         <v>0</v>
       </c>
       <c r="L20" s="37"/>
@@ -1805,16 +1805,16 @@
       <c r="B21" s="23"/>
       <c r="C21" s="24"/>
       <c r="D21" s="31" t="n">
-        <f aca="false">IF(E21=0,0,IF(C21&gt;0,(C21-C20)/100,0))</f>
+        <f aca="false">IF(A21="",0,IF(C21&gt;0,(C21-C20)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E21" s="36"/>
       <c r="F21" s="33" t="n">
-        <f aca="false">IF(E21=0,0,IF(J21&lt;-20,-D21/1.5+E21,IF(J21&lt;0,E21,D21+E21)))</f>
+        <f aca="false">IF(A21="",0,IF(J21&lt;-20,-D21/1.5+E21,IF(J21&lt;0,E21,D21+E21)))</f>
         <v>0</v>
       </c>
       <c r="G21" s="34" t="n">
-        <f aca="false">IF(E21=0,0,TIME(0,60/$N$3*F21,0))</f>
+        <f aca="false">IF(A21="",0,TIME(0,60/$N$3*F21,0))</f>
         <v>0</v>
       </c>
       <c r="H21" s="33" t="n">
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="35" t="n">
-        <f aca="false">IF((K20+G21+M21)&lt;&gt;K20,K20+G21+M21,0)</f>
+        <f aca="false">K20+G21+M21</f>
         <v>0</v>
       </c>
       <c r="L21" s="37"/>
@@ -1842,16 +1842,16 @@
       <c r="B22" s="23"/>
       <c r="C22" s="24"/>
       <c r="D22" s="31" t="n">
-        <f aca="false">IF(E22=0,0,IF(C22&gt;0,(C22-C21)/100,0))</f>
+        <f aca="false">IF(A22="",0,IF(C22&gt;0,(C22-C21)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E22" s="36"/>
       <c r="F22" s="33" t="n">
-        <f aca="false">IF(E22=0,0,IF(J22&lt;-20,-D22/1.5+E22,IF(J22&lt;0,E22,D22+E22)))</f>
+        <f aca="false">IF(A22="",0,IF(J22&lt;-20,-D22/1.5+E22,IF(J22&lt;0,E22,D22+E22)))</f>
         <v>0</v>
       </c>
       <c r="G22" s="34" t="n">
-        <f aca="false">IF(E22=0,0,TIME(0,60/$N$3*F22,0))</f>
+        <f aca="false">IF(A22="",0,TIME(0,60/$N$3*F22,0))</f>
         <v>0</v>
       </c>
       <c r="H22" s="33" t="n">
@@ -1867,7 +1867,7 @@
         <v>0</v>
       </c>
       <c r="K22" s="35" t="n">
-        <f aca="false">IF((K21+G22+M22)&lt;&gt;K21,K21+G22+M22,0)</f>
+        <f aca="false">K21+G22+M22</f>
         <v>0</v>
       </c>
       <c r="L22" s="37"/>
@@ -1879,16 +1879,16 @@
       <c r="B23" s="23"/>
       <c r="C23" s="24"/>
       <c r="D23" s="31" t="n">
-        <f aca="false">IF(E23=0,0,IF(C23&gt;0,(C23-C22)/100,0))</f>
+        <f aca="false">IF(A23="",0,IF(C23&gt;0,(C23-C22)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="33" t="n">
-        <f aca="false">IF(E23=0,0,IF(J23&lt;-20,-D23/1.5+E23,IF(J23&lt;0,E23,D23+E23)))</f>
+        <f aca="false">IF(A23="",0,IF(J23&lt;-20,-D23/1.5+E23,IF(J23&lt;0,E23,D23+E23)))</f>
         <v>0</v>
       </c>
       <c r="G23" s="34" t="n">
-        <f aca="false">IF(E23=0,0,TIME(0,60/$N$3*F23,0))</f>
+        <f aca="false">IF(A23="",0,TIME(0,60/$N$3*F23,0))</f>
         <v>0</v>
       </c>
       <c r="H23" s="33" t="n">
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="35" t="n">
-        <f aca="false">IF((K22+G23+M23)&lt;&gt;K22,K22+G23+M23,0)</f>
+        <f aca="false">K22+G23+M23</f>
         <v>0</v>
       </c>
       <c r="L23" s="37"/>
@@ -1916,16 +1916,16 @@
       <c r="B24" s="23"/>
       <c r="C24" s="24"/>
       <c r="D24" s="31" t="n">
-        <f aca="false">IF(E24=0,0,IF(C24&gt;0,(C24-C23)/100,0))</f>
+        <f aca="false">IF(A24="",0,IF(C24&gt;0,(C24-C23)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E24" s="36"/>
       <c r="F24" s="33" t="n">
-        <f aca="false">IF(E24=0,0,IF(J24&lt;-20,-D24/1.5+E24,IF(J24&lt;0,E24,D24+E24)))</f>
+        <f aca="false">IF(A24="",0,IF(J24&lt;-20,-D24/1.5+E24,IF(J24&lt;0,E24,D24+E24)))</f>
         <v>0</v>
       </c>
       <c r="G24" s="34" t="n">
-        <f aca="false">IF(E24=0,0,TIME(0,60/$N$3*F24,0))</f>
+        <f aca="false">IF(A24="",0,TIME(0,60/$N$3*F24,0))</f>
         <v>0</v>
       </c>
       <c r="H24" s="33" t="n">
@@ -1941,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="35" t="n">
-        <f aca="false">IF((K23+G24+M24)&lt;&gt;K23,K23+G24+M24,0)</f>
+        <f aca="false">K23+G24+M24</f>
         <v>0</v>
       </c>
       <c r="L24" s="37"/>
@@ -1953,16 +1953,16 @@
       <c r="B25" s="23"/>
       <c r="C25" s="24"/>
       <c r="D25" s="31" t="n">
-        <f aca="false">IF(E25=0,0,IF(C25&gt;0,(C25-C24)/100,0))</f>
+        <f aca="false">IF(A25="",0,IF(C25&gt;0,(C25-C24)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E25" s="36"/>
       <c r="F25" s="33" t="n">
-        <f aca="false">IF(E25=0,0,IF(J25&lt;-20,-D25/1.5+E25,IF(J25&lt;0,E25,D25+E25)))</f>
+        <f aca="false">IF(A25="",0,IF(J25&lt;-20,-D25/1.5+E25,IF(J25&lt;0,E25,D25+E25)))</f>
         <v>0</v>
       </c>
       <c r="G25" s="34" t="n">
-        <f aca="false">IF(E25=0,0,TIME(0,60/$N$3*F25,0))</f>
+        <f aca="false">IF(A25="",0,TIME(0,60/$N$3*F25,0))</f>
         <v>0</v>
       </c>
       <c r="H25" s="33" t="n">
@@ -1978,7 +1978,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="35" t="n">
-        <f aca="false">IF((K24+G25+M25)&lt;&gt;K24,K24+G25+M25,0)</f>
+        <f aca="false">K24+G25+M25</f>
         <v>0</v>
       </c>
       <c r="L25" s="37"/>
@@ -1990,16 +1990,16 @@
       <c r="B26" s="23"/>
       <c r="C26" s="24"/>
       <c r="D26" s="31" t="n">
-        <f aca="false">IF(E26=0,0,IF(C26&gt;0,(C26-C25)/100,0))</f>
+        <f aca="false">IF(A26="",0,IF(C26&gt;0,(C26-C25)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E26" s="36"/>
       <c r="F26" s="33" t="n">
-        <f aca="false">IF(E26=0,0,IF(J26&lt;-20,-D26/1.5+E26,IF(J26&lt;0,E26,D26+E26)))</f>
+        <f aca="false">IF(A26="",0,IF(J26&lt;-20,-D26/1.5+E26,IF(J26&lt;0,E26,D26+E26)))</f>
         <v>0</v>
       </c>
       <c r="G26" s="34" t="n">
-        <f aca="false">IF(E26=0,0,TIME(0,60/$N$3*F26,0))</f>
+        <f aca="false">IF(A26="",0,TIME(0,60/$N$3*F26,0))</f>
         <v>0</v>
       </c>
       <c r="H26" s="33" t="n">
@@ -2015,7 +2015,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="35" t="n">
-        <f aca="false">IF((K25+G26+M26)&lt;&gt;K25,K25+G26+M26,0)</f>
+        <f aca="false">K25+G26+M26</f>
         <v>0</v>
       </c>
       <c r="L26" s="37"/>
@@ -2027,16 +2027,16 @@
       <c r="B27" s="23"/>
       <c r="C27" s="24"/>
       <c r="D27" s="31" t="n">
-        <f aca="false">IF(E27=0,0,IF(C27&gt;0,(C27-C26)/100,0))</f>
+        <f aca="false">IF(A27="",0,IF(C27&gt;0,(C27-C26)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="33" t="n">
-        <f aca="false">IF(E27=0,0,IF(J27&lt;-20,-D27/1.5+E27,IF(J27&lt;0,E27,D27+E27)))</f>
+        <f aca="false">IF(A27="",0,IF(J27&lt;-20,-D27/1.5+E27,IF(J27&lt;0,E27,D27+E27)))</f>
         <v>0</v>
       </c>
       <c r="G27" s="34" t="n">
-        <f aca="false">IF(E27=0,0,TIME(0,60/$N$3*F27,0))</f>
+        <f aca="false">IF(A27="",0,TIME(0,60/$N$3*F27,0))</f>
         <v>0</v>
       </c>
       <c r="H27" s="33" t="n">
@@ -2052,7 +2052,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="35" t="n">
-        <f aca="false">IF((K26+G27+M27)&lt;&gt;K26,K26+G27+M27,0)</f>
+        <f aca="false">K26+G27+M27</f>
         <v>0</v>
       </c>
       <c r="L27" s="37"/>
@@ -2064,16 +2064,16 @@
       <c r="B28" s="23"/>
       <c r="C28" s="24"/>
       <c r="D28" s="31" t="n">
-        <f aca="false">IF(E28=0,0,IF(C28&gt;0,(C28-C27)/100,0))</f>
+        <f aca="false">IF(A28="",0,IF(C28&gt;0,(C28-C27)/100,0))</f>
         <v>0</v>
       </c>
       <c r="E28" s="36"/>
       <c r="F28" s="33" t="n">
-        <f aca="false">IF(E28=0,0,IF(J28&lt;-20,-D28/1.5+E28,IF(J28&lt;0,E28,D28+E28)))</f>
+        <f aca="false">IF(A28="",0,IF(J28&lt;-20,-D28/1.5+E28,IF(J28&lt;0,E28,D28+E28)))</f>
         <v>0</v>
       </c>
       <c r="G28" s="34" t="n">
-        <f aca="false">IF(E28=0,0,TIME(0,60/$N$3*F28,0))</f>
+        <f aca="false">IF(A28="",0,TIME(0,60/$N$3*F28,0))</f>
         <v>0</v>
       </c>
       <c r="H28" s="33" t="n">
@@ -2089,7 +2089,7 @@
         <v>0</v>
       </c>
       <c r="K28" s="35" t="n">
-        <f aca="false">IF((K27+G28+M28)&lt;&gt;K27,K27+G28+M28,0)</f>
+        <f aca="false">K27+G28+M28</f>
         <v>0</v>
       </c>
       <c r="L28" s="37"/>

</xml_diff>